<commit_message>
working up to small test scenario 6 + replaced wav files for working loop
</commit_message>
<xml_diff>
--- a/sm2.xlsx
+++ b/sm2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="15135" windowHeight="5580"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -383,7 +383,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>